<commit_message>
All of the tests for dancing links
</commit_message>
<xml_diff>
--- a/phase 3/testing.xlsx
+++ b/phase 3/testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steem\Desktop\studie\project 1-1 group 25\phase 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01B722FA-C8BA-403A-AF7B-4C9DCEA45460}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2718DBC1-FB29-4A6C-9D4C-02A9C630528B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2988" yWindow="2172" windowWidth="20292" windowHeight="9120"/>
+    <workbookView xWindow="2328" yWindow="2016" windowWidth="20292" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>B</t>
   </si>
@@ -42,19 +42,124 @@
     <t>Time</t>
   </si>
   <si>
-    <t>30s</t>
-  </si>
-  <si>
-    <t>1h</t>
-  </si>
-  <si>
-    <t>Normal version with pruning pruneWait = 3; pruneCutoff = .85F; layerCutoff = 15;</t>
+    <t>5s</t>
+  </si>
+  <si>
+    <t>20s</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>10m</t>
+  </si>
+  <si>
+    <t>PruneWaits</t>
+  </si>
+  <si>
+    <t>Different pruneWaits for 5 seconds</t>
+  </si>
+  <si>
+    <t>Different pruneCutoffs for 5 seconds</t>
+  </si>
+  <si>
+    <t>.7</t>
+  </si>
+  <si>
+    <t>.9</t>
+  </si>
+  <si>
+    <t>Different layerCutoff for 5 seconds</t>
+  </si>
+  <si>
+    <t>If not specified the values used are pruneWait=3; pruneCutoff=.85; layerCutoff=15; maxTime=10</t>
+  </si>
+  <si>
+    <t>Normal version with pruning pruneWait = 3; pruneCutoff = .85; layerCutoff = 15;</t>
+  </si>
+  <si>
+    <t>pruneWait</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>The amount of branches that will be skipped after each time pruning occurs</t>
+  </si>
+  <si>
+    <t>pruneCutoff</t>
+  </si>
+  <si>
+    <t>The multiplier for the maximum score that is used. If the score for the current solution is below this than this branch is discontinued.</t>
+  </si>
+  <si>
+    <t>layerCutoff</t>
+  </si>
+  <si>
+    <t>Up to which layer pruning will not occur.</t>
+  </si>
+  <si>
+    <t>maxTime</t>
+  </si>
+  <si>
+    <t>The amount of seconds that the algorithm has to run (excluding setting up the structure, getting the input and updating UI)</t>
+  </si>
+  <si>
+    <t>1s</t>
+  </si>
+  <si>
+    <t>All tests were run on a laptop with the following specs:</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>STORAGE</t>
+  </si>
+  <si>
+    <t>i7-7700HQ 4 cores with hypertreading at 2.8 Ghz</t>
+  </si>
+  <si>
+    <t>M.2 SSD</t>
+  </si>
+  <si>
+    <t>16GB 2400MHz</t>
+  </si>
+  <si>
+    <t>The exact model is HP Omen 15-ce032nd</t>
+  </si>
+  <si>
+    <t>pruneCutoffs</t>
+  </si>
+  <si>
+    <t>.1</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>Greedy</t>
+  </si>
+  <si>
+    <t>Pruning with greedy</t>
+  </si>
+  <si>
+    <t>Pruning without greedy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,51 +504,435 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>236</v>
+      </c>
+      <c r="E19">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>236</v>
+      </c>
+      <c r="E20">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>236</v>
+      </c>
+      <c r="E21">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C22">
+        <v>236</v>
+      </c>
+      <c r="E22">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>236</v>
+      </c>
+      <c r="E23">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E26" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>233</v>
+      </c>
+      <c r="E27">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C28">
+        <v>236</v>
+      </c>
+      <c r="E28">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>236</v>
+      </c>
+      <c r="E29">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>50</v>
+      </c>
+      <c r="C30">
+        <v>236</v>
+      </c>
+      <c r="E30">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34">
+        <v>236</v>
+      </c>
+      <c r="E34">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>236</v>
+      </c>
+      <c r="E35">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>233</v>
+      </c>
+      <c r="E36">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>224</v>
+      </c>
+      <c r="E37">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>236</v>
+      </c>
+      <c r="E41">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>236</v>
+      </c>
+      <c r="E42">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>20</v>
+      </c>
+      <c r="C43">
+        <v>236</v>
+      </c>
+      <c r="E43">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46">
+        <v>236</v>
+      </c>
+      <c r="E46">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47">
+        <v>236</v>
+      </c>
+      <c r="E47">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50">
         <v>228</v>
       </c>
-      <c r="E3">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
+      <c r="E50">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51">
         <v>228</v>
       </c>
-      <c r="E4">
-        <v>842</v>
+      <c r="E51">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54">
+        <v>236</v>
+      </c>
+      <c r="E54">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>37</v>
+      </c>
+      <c r="C55">
+        <v>228</v>
+      </c>
+      <c r="E55">
+        <v>834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>